<commit_message>
create a new file
</commit_message>
<xml_diff>
--- a/Google.xlsx
+++ b/Google.xlsx
@@ -477,17 +477,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>https://ru.wikipedia.org/wiki/%D0%AF%D0%B1%D0%BB%D0%BE%D0%BA%D0%BE_(%D0%BF%D0%B0%D1%80%D1%82%D0%B8%D1%8F)</t>
+          <t>https://www.apple.com/ru/</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Яблоко (партия) — Википедия</t>
+          <t>Apple (Россия) – Официальный сайт</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>Российская объединённая демократическая партия «Яблоко» — зарегистрированная российская политическая партия центристского и ...</t>
+          <t>Все инновации Apple, включая iPhone, iPad, Apple Watch, Mac, Apple TV. А также аксессуары, развлечения, справочная информация и многое другое.</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
@@ -497,17 +497,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>https://ru.wikipedia.org/wiki/%D0%AF%D0%B1%D0%BB%D0%BE%D0%BA%D0%BE</t>
+          <t>https://ru.wikipedia.org/wiki/%D0%AF%D0%B1%D0%BB%D0%BE%D0%BA%D0%BE_(%D0%BF%D0%B0%D1%80%D1%82%D0%B8%D1%8F)</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Яблоко — Википедия</t>
+          <t>Яблоко (партия) — Википедия</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>Я́блоко — сочный плод яблони, который употребляется в пищу в свежем виде, служит сырьём в кулинарии и для приготовления напитков. Наибольшее ...</t>
+          <t>Российская объединённая демократическая партия «Яблоко» — зарегистрированная российская политическая партия центристского и ...</t>
         </is>
       </c>
       <c r="D4" s="1" t="n">
@@ -517,17 +517,17 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>https://www.apple.com/ru/</t>
+          <t>https://ru.wikipedia.org/wiki/%D0%AF%D0%B1%D0%BB%D0%BE%D0%BA%D0%BE</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Apple (Россия) – Официальный сайт</t>
+          <t>Яблоко — Википедия</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>Все инновации Apple, включая iPhone, iPad, Apple Watch, Mac, Apple TV. А также аксессуары, развлечения, справочная информация и многое другое.</t>
+          <t>Я́блоко — сочный плод яблони, который употребляется в пищу в свежем виде, служит сырьём в кулинарии и для приготовления напитков. Наибольшее ...</t>
         </is>
       </c>
       <c r="D5" s="1" t="n">
@@ -537,17 +537,17 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>https://www.apple.com/ru/iphone/</t>
+          <t>https://goldapple.ru/</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>iPhone – Apple (RU)</t>
+          <t>«Золотое яблоко» - интернет-магазин косметики и ...</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>iPhone 11 Pro, iPhone 11 Pro Max, iPhone 11, iPhone SE и iPhone XR — всё это iPhone, невероятно мощное персональное устройство.</t>
+          <t>Косметика и парфюмерия — купите онлайн в интернет-магазине «Золотое яблоко». Более 700 известных брендов: профессиональная, натуральная, ...</t>
         </is>
       </c>
       <c r="D6" s="1" t="n">
@@ -557,17 +557,17 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>https://goldapple.ru/</t>
+          <t>https://vk.com/yabloko_ru</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>«Золотое яблоко» - интернет-магазин косметики и ...</t>
+          <t>Партия ЯБЛОКО | ВКонтакте</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>Косметика и парфюмерия — купите онлайн в интернет-магазине «Золотое яблоко». Более 700 известных брендов: профессиональная, натуральная, ...</t>
+          <t>Российская объединенная демократическая партия ЯБЛОКО Мы боремся за то, чтобы сделать Россию сильной и современной страной, удобной и ...</t>
         </is>
       </c>
       <c r="D7" s="1" t="n">
@@ -577,17 +577,17 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>https://vk.com/yabloko_ru</t>
+          <t>https://mosyabloko.ru/</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Партия ЯБЛОКО | ВКонтакте</t>
+          <t>Московское ЯБЛОКО: Главная</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>Российская объединенная демократическая партия ЯБЛОКО Мы боремся за то, чтобы сделать Россию сильной и современной страной, удобной и ...</t>
+          <t>В Марьино от партии «Яблоко» на дополнительных выборах в Совет депутатов будут баллотироваться Сергей Запольнов и Данила Столь.</t>
         </is>
       </c>
       <c r="D8" s="1" t="n">
@@ -597,17 +597,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>https://mosyabloko.ru/</t>
+          <t>https://lenta.ru/lib/14159780/</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>Московское ЯБЛОКО: Главная</t>
+          <t>РОДП Яблоко - Lenta.ru</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>В Марьино от партии «Яблоко» на дополнительных выборах в Совет депутатов будут баллотироваться Сергей Запольнов и Данила Столь.</t>
+          <t>Имела фракцию в нескольких составах Государственной думы в 1993-2003 годах. Российская объединенная демократическая партия "Яблоко" ...</t>
         </is>
       </c>
       <c r="D9" s="1" t="n">
@@ -617,17 +617,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>https://lenta.ru/lib/14159780/</t>
+          <t>https://ria.ru/organization_JAbloko/</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>РОДП Яблоко - Lenta.ru</t>
+          <t>Яблоко - последние новости сегодня - РИА Новости</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>Имела фракцию в нескольких составах Государственной думы в 1993-2003 годах. Российская объединенная демократическая партия "Яблоко" ...</t>
+          <t>Яблоко. Читайте последние новости на тему в ленте новостей на сайте РИА Новости. Сенатор Алексей Пушков прокомментировал предложение Яна ...</t>
         </is>
       </c>
       <c r="D10" s="1" t="n">
@@ -637,17 +637,17 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>https://ria.ru/organization_JAbloko/</t>
+          <t>https://ru.wikiquote.org/wiki/%D0%AF%D0%B1%D0%BB%D0%BE%D0%BA%D0%BE</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>Яблоко - последние новости сегодня - РИА Новости</t>
+          <t>Яблоко — Викицитатник</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>Яблоко. Читайте последние новости на тему в ленте новостей на сайте РИА Новости. Сенатор Алексей Пушков прокомментировал предложение Яна ...</t>
+          <t>Я́блоко — съедобный плод яблони, который употребляют в пищу как в свежем, так и в приготовленном виде: сушёном, мочёном, квашеном, печёном, ...</t>
         </is>
       </c>
       <c r="D11" s="1" t="n">
@@ -806,8 +806,16 @@
           <t>https://foodandmood.com.ua/rid/food/708324-chem-polezen-i-opasen-abrikos</t>
         </is>
       </c>
-      <c r="B7" s="1" t="inlineStr"/>
-      <c r="C7" s="1" t="inlineStr"/>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Чем полезен и опасен абрикос - foodandmood.com.ua</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>Выбирайте упругие абрикосы, без повреждений и вмятин. Спелый абрикос очень ароматный и имеет ровную окраску. Избегайте абрикосов с темными ...</t>
+        </is>
+      </c>
       <c r="D7" s="1" t="n">
         <v>6</v>
       </c>
@@ -815,7 +823,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>https://otvet.mail.ru/question/49528960</t>
+          <t>https://foodandmood.com.ua/rid/food/708324-chem-polezen-i-opasen-abrikos</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr"/>
@@ -827,7 +835,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>https://yandex.ru/znatoki/question/garden/chem_otlichaetsia_sliva_ot_abrikosa_82ccaacb/</t>
+          <t>https://otvet.mail.ru/question/49528960</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr"/>
@@ -839,7 +847,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>https://forum.derev-grad.ru/plodovie-derevya-f94/skol-ko-let-zhivut-derev-ya-t6442.html</t>
+          <t>https://yandex.ru/znatoki/question/garden/chem_otlichaetsia_sliva_ot_abrikosa_82ccaacb/</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr"/>
@@ -851,19 +859,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>https://foodandmood.com.ua/rid/food/708324-chem-polezen-i-opasen-abrikos</t>
-        </is>
-      </c>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>Чем полезен и опасен абрикос - foodandmood.com.ua</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="inlineStr">
-        <is>
-          <t>Выбирайте упругие абрикосы, без повреждений и вмятин. Спелый абрикос очень ароматный и имеет ровную окраску. Избегайте абрикосов с темными ...</t>
-        </is>
-      </c>
+          <t>https://forum.derev-grad.ru/plodovie-derevya-f94/skol-ko-let-zhivut-derev-ya-t6442.html</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr"/>
+      <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="n">
         <v>10</v>
       </c>

</xml_diff>